<commit_message>
Company import updated with GST number
</commit_message>
<xml_diff>
--- a/public/files/Register_Company.xlsx
+++ b/public/files/Register_Company.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\groemp\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5FF8FB-7229-461C-83C9-89F53A53479F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F39552-F97A-4DEA-960E-42D4E37EA59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="dlDXtaoofBd1AL5BFN6H8yaEFFxGaukZKUiNmIQxd0HwO/U0nBTY0YoiKRK+fLVLrls+aSnwQs2uhVsy9mqOjg==" workbookSaltValue="Wy8bbh0WmU/HAJjdNMXFig==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{02B70855-7806-477B-96D9-635DA2BB080B}"/>
@@ -45,28 +45,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -81,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="240">
   <si>
     <t>Group_Company_PAN</t>
   </si>
@@ -795,6 +786,12 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>GST No</t>
+  </si>
+  <si>
+    <t>Error in GST No</t>
   </si>
 </sst>
 </file>
@@ -1031,13 +1028,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1133475</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>31946</xdr:rowOff>
@@ -1373,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859E83F7-58AE-478B-A308-ACEDC2633004}">
-  <dimension ref="A1:AA34"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H7"/>
+      <selection activeCell="A2" sqref="A2:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1385,26 +1382,26 @@
     <col min="2" max="2" width="17.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="9" width="3.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.81640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="1"/>
-    <col min="14" max="14" width="22" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.81640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="20.54296875" style="1" customWidth="1"/>
-    <col min="17" max="18" width="20.26953125" style="1" customWidth="1"/>
-    <col min="19" max="21" width="9.1796875" style="1"/>
-    <col min="22" max="22" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="15.54296875" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="6" width="30.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.453125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.81640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.1796875" style="1"/>
+    <col min="15" max="15" width="22" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.81640625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="20.54296875" style="1" customWidth="1"/>
+    <col min="19" max="21" width="20.26953125" style="1" customWidth="1"/>
+    <col min="22" max="24" width="9.1796875" style="1"/>
+    <col min="25" max="25" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="15.54296875" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>237</v>
       </c>
@@ -1421,67 +1418,77 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="8" t="str">
+      <c r="O1" s="8" t="str">
         <f>+"Duplicate "&amp;A1&amp;" Error"</f>
         <v>Duplicate Name Error</v>
       </c>
-      <c r="O1" s="8" t="str">
+      <c r="P1" s="8" t="str">
         <f>+"Duplicate "&amp;C1&amp;" Error"</f>
         <v>Duplicate PAN Error</v>
       </c>
-      <c r="P1" s="8" t="str">
+      <c r="Q1" s="8" t="str">
         <f>+"Duplicate "&amp;D1&amp;" Error"</f>
         <v>Duplicate Admin_Mobile Error</v>
       </c>
-      <c r="Q1" s="8" t="str">
+      <c r="R1" s="8" t="str">
+        <f>+"Duplicate "&amp;F1&amp;" Error"</f>
+        <v>Duplicate GST No Error</v>
+      </c>
+      <c r="S1" s="8" t="str">
         <f>+"Duplicate "&amp;E1&amp;" Error"</f>
         <v>Duplicate Admin_Email Error</v>
       </c>
-      <c r="R1" s="8" t="str">
+      <c r="T1" s="8" t="str">
         <f>"Error in "&amp;D1</f>
         <v>Error in Admin_Mobile</v>
       </c>
-      <c r="S1" s="8" t="str">
-        <f>"Error in "&amp;H1</f>
+      <c r="U1" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="V1" s="8" t="str">
+        <f>"Error in "&amp;I1</f>
         <v>Error in Pincode</v>
       </c>
-      <c r="U1" s="8" t="str">
+      <c r="X1" s="8" t="str">
         <f>A1</f>
         <v>Name</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="W1" s="8" t="str">
+      <c r="Z1" s="8" t="str">
         <f>+D1</f>
         <v>Admin_Mobile</v>
       </c>
-      <c r="X1" s="8" t="str">
+      <c r="AA1" s="8" t="str">
         <f>+E1</f>
         <v>Admin_Email</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="AA1" s="8">
+      <c r="AD1" s="8">
         <v>123456</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1489,45 +1496,50 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="1">
-        <f>+COUNTIF(N2:S34,FALSE)</f>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="1">
+        <f>+COUNTIF(O2:V34,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="L2" s="1" t="str">
-        <f>IF(F2="","",+VLOOKUP(F2,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
       <c r="M2" s="1" t="str">
-        <f>IF(G2="","",+VLOOKUP(G2,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="R2" s="1" t="str">
+        <f>IF(G2="","",+VLOOKUP(G2,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f>IF(H2="","",+VLOOKUP(H2,'STD Code'!$A$1:$B$150,2,0))</f>
+        <v/>
+      </c>
+      <c r="T2" s="1" t="str">
         <f>IF(D2="","",IF(AND(D2&lt;9999999999,D2&gt;1000000000),"",FALSE))</f>
         <v/>
       </c>
-      <c r="S2" s="1" t="str">
-        <f>IF(H2="","",IF(AND(H2&lt;999999,H2&gt;100000),"",FALSE))</f>
-        <v/>
-      </c>
       <c r="U2" s="1" t="str">
-        <f>+A2&amp;F2</f>
+        <f>IF(F2="","",IF(AND((LEFT(F2,2)/1=G2),MID(F2,3,10)=C2),"",FALSE))</f>
         <v/>
       </c>
       <c r="V2" s="1" t="str">
-        <f>+C2&amp;F2</f>
-        <v/>
-      </c>
-      <c r="W2" s="1" t="str">
-        <f>+D2&amp;F2</f>
+        <f>IF(I2="","",IF(AND(I2&lt;999999,I2&gt;100000),"",FALSE))</f>
         <v/>
       </c>
       <c r="X2" s="1" t="str">
-        <f>+E2&amp;F2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+        <f>+A2&amp;G2</f>
+        <v/>
+      </c>
+      <c r="Y2" s="1" t="str">
+        <f>+C2&amp;G2</f>
+        <v/>
+      </c>
+      <c r="Z2" s="1" t="str">
+        <f>+D2&amp;G2</f>
+        <v/>
+      </c>
+      <c r="AA2" s="1" t="str">
+        <f>+E2&amp;G2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1535,57 +1547,66 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="L3" s="1" t="str">
-        <f>IF(F3="","",+VLOOKUP(F3,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
       <c r="M3" s="1" t="str">
-        <f>IF(G3="","",+VLOOKUP(G3,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N3" s="1" t="str" cm="1">
-        <f t="array" ref="N3">IF(U3="","",IF(AND(U3&lt;&gt;U$2:U2),"",FALSE))</f>
+        <f>IF(G3="","",+VLOOKUP(G3,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f>IF(H3="","",+VLOOKUP(H3,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O3" s="1" t="str" cm="1">
-        <f t="array" ref="O3">IF(V3="","",IF(AND(V3&lt;&gt;V$2:V2),"",FALSE))</f>
+        <f t="array" ref="O3">IF(X3="","",IF(AND(X3&lt;&gt;X$2:X2),"",FALSE))</f>
         <v/>
       </c>
       <c r="P3" s="1" t="str" cm="1">
-        <f t="array" ref="P3">IF(W3="","",IF(AND(W3&lt;&gt;W$2:W2),"",FALSE))</f>
+        <f t="array" ref="P3">IF(Y3="","",IF(AND(Y3&lt;&gt;Y$2:Y2),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q3" s="1" t="str" cm="1">
-        <f t="array" ref="Q3">IF(X3="","",IF(AND(X3&lt;&gt;X$2:X2),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R3" s="1" t="str">
-        <f t="shared" ref="R3:R34" si="0">IF(D3="","",IF(AND(D3&lt;9999999999,D3&gt;1000000000),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="S3" s="1" t="str">
-        <f t="shared" ref="S3:S34" si="1">IF(H3="","",IF(AND(H3&lt;999999,H3&gt;100000),"",FALSE))</f>
+        <f t="array" ref="Q3">IF(Z3="","",IF(AND(Z3&lt;&gt;Z$2:Z2),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R3" s="1" t="str" cm="1">
+        <f t="array" ref="R3">IF(F3="","",IF(AND(F3&lt;&gt;F$2:F2),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S3" s="1" t="str" cm="1">
+        <f t="array" ref="S3">IF(AA3="","",IF(AND(AA3&lt;&gt;AA$2:AA2),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T3" s="1" t="str">
+        <f t="shared" ref="T3:T34" si="0">IF(D3="","",IF(AND(D3&lt;9999999999,D3&gt;1000000000),"",FALSE))</f>
         <v/>
       </c>
       <c r="U3" s="1" t="str">
-        <f t="shared" ref="U3:U34" si="2">+A3&amp;F3</f>
+        <f t="shared" ref="U3:U34" si="1">IF(F3="","",IF(AND((LEFT(F3,2)/1=G3),MID(F3,3,10)=C3),"",FALSE))</f>
         <v/>
       </c>
       <c r="V3" s="1" t="str">
-        <f t="shared" ref="V3:V34" si="3">+C3&amp;F3</f>
-        <v/>
-      </c>
-      <c r="W3" s="1" t="str">
-        <f t="shared" ref="W3:W34" si="4">+D3&amp;F3</f>
+        <f>IF(I3="","",IF(AND(I3&lt;999999,I3&gt;100000),"",FALSE))</f>
         <v/>
       </c>
       <c r="X3" s="1" t="str">
-        <f t="shared" ref="X3:X34" si="5">+E3&amp;F3</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+        <f>+A3&amp;G3</f>
+        <v/>
+      </c>
+      <c r="Y3" s="1" t="str">
+        <f>+C3&amp;G3</f>
+        <v/>
+      </c>
+      <c r="Z3" s="1" t="str">
+        <f>+D3&amp;G3</f>
+        <v/>
+      </c>
+      <c r="AA3" s="1" t="str">
+        <f>+E3&amp;G3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1593,57 +1614,66 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="L4" s="1" t="str">
-        <f>IF(F4="","",+VLOOKUP(F4,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
       <c r="M4" s="1" t="str">
-        <f>IF(G4="","",+VLOOKUP(G4,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N4" s="1" t="str" cm="1">
-        <f t="array" ref="N4">IF(U4="","",IF(AND(U4&lt;&gt;U$2:U3),"",FALSE))</f>
+        <f>IF(G4="","",+VLOOKUP(G4,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f>IF(H4="","",+VLOOKUP(H4,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O4" s="1" t="str" cm="1">
-        <f t="array" ref="O4">IF(V4="","",IF(AND(V4&lt;&gt;V$2:V3),"",FALSE))</f>
+        <f t="array" ref="O4">IF(X4="","",IF(AND(X4&lt;&gt;X$2:X3),"",FALSE))</f>
         <v/>
       </c>
       <c r="P4" s="1" t="str" cm="1">
-        <f t="array" ref="P4">IF(W4="","",IF(AND(W4&lt;&gt;W$2:W3),"",FALSE))</f>
+        <f t="array" ref="P4">IF(Y4="","",IF(AND(Y4&lt;&gt;Y$2:Y3),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q4" s="1" t="str" cm="1">
-        <f t="array" ref="Q4">IF(X4="","",IF(AND(X4&lt;&gt;X$2:X3),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R4" s="1" t="str">
+        <f t="array" ref="Q4">IF(Z4="","",IF(AND(Z4&lt;&gt;Z$2:Z3),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R4" s="1" t="str" cm="1">
+        <f t="array" ref="R4">IF(F4="","",IF(AND(F4&lt;&gt;F$2:F3),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S4" s="1" t="str" cm="1">
+        <f t="array" ref="S4">IF(AA4="","",IF(AND(AA4&lt;&gt;AA$2:AA3),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T4" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S4" s="1" t="str">
+      <c r="U4" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="V4" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="W4" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(I4="","",IF(AND(I4&lt;999999,I4&gt;100000),"",FALSE))</f>
         <v/>
       </c>
       <c r="X4" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+        <f>+A4&amp;G4</f>
+        <v/>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <f>+C4&amp;G4</f>
+        <v/>
+      </c>
+      <c r="Z4" s="1" t="str">
+        <f>+D4&amp;G4</f>
+        <v/>
+      </c>
+      <c r="AA4" s="1" t="str">
+        <f>+E4&amp;G4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1651,57 +1681,66 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="L5" s="1" t="str">
-        <f>IF(F5="","",+VLOOKUP(F5,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
       <c r="M5" s="1" t="str">
-        <f>IF(G5="","",+VLOOKUP(G5,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N5" s="1" t="str" cm="1">
-        <f t="array" ref="N5">IF(U5="","",IF(AND(U5&lt;&gt;U$2:U4),"",FALSE))</f>
+        <f>IF(G5="","",+VLOOKUP(G5,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f>IF(H5="","",+VLOOKUP(H5,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O5" s="1" t="str" cm="1">
-        <f t="array" ref="O5">IF(V5="","",IF(AND(V5&lt;&gt;V$2:V4),"",FALSE))</f>
+        <f t="array" ref="O5">IF(X5="","",IF(AND(X5&lt;&gt;X$2:X4),"",FALSE))</f>
         <v/>
       </c>
       <c r="P5" s="1" t="str" cm="1">
-        <f t="array" ref="P5">IF(W5="","",IF(AND(W5&lt;&gt;W$2:W4),"",FALSE))</f>
+        <f t="array" ref="P5">IF(Y5="","",IF(AND(Y5&lt;&gt;Y$2:Y4),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q5" s="1" t="str" cm="1">
-        <f t="array" ref="Q5">IF(X5="","",IF(AND(X5&lt;&gt;X$2:X4),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R5" s="1" t="str">
+        <f t="array" ref="Q5">IF(Z5="","",IF(AND(Z5&lt;&gt;Z$2:Z4),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R5" s="1" t="str" cm="1">
+        <f t="array" ref="R5">IF(F5="","",IF(AND(F5&lt;&gt;F$2:F4),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S5" s="1" t="str" cm="1">
+        <f t="array" ref="S5">IF(AA5="","",IF(AND(AA5&lt;&gt;AA$2:AA4),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T5" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S5" s="1" t="str">
+      <c r="U5" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="V5" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="W5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="V5:V34" si="2">IF(I5="","",IF(AND(I5&lt;999999,I5&gt;100000),"",FALSE))</f>
         <v/>
       </c>
       <c r="X5" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+        <f t="shared" ref="X5:X34" si="3">+A5&amp;G5</f>
+        <v/>
+      </c>
+      <c r="Y5" s="1" t="str">
+        <f t="shared" ref="Y5:Y34" si="4">+C5&amp;G5</f>
+        <v/>
+      </c>
+      <c r="Z5" s="1" t="str">
+        <f t="shared" ref="Z5:Z34" si="5">+D5&amp;G5</f>
+        <v/>
+      </c>
+      <c r="AA5" s="1" t="str">
+        <f t="shared" ref="AA5:AA34" si="6">+E5&amp;G5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1709,57 +1748,66 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="L6" s="1" t="str">
-        <f>IF(F6="","",+VLOOKUP(F6,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
       <c r="M6" s="1" t="str">
-        <f>IF(G6="","",+VLOOKUP(G6,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N6" s="1" t="str" cm="1">
-        <f t="array" ref="N6">IF(U6="","",IF(AND(U6&lt;&gt;U$2:U5),"",FALSE))</f>
+        <f>IF(G6="","",+VLOOKUP(G6,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f>IF(H6="","",+VLOOKUP(H6,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O6" s="1" t="str" cm="1">
-        <f t="array" ref="O6">IF(V6="","",IF(AND(V6&lt;&gt;V$2:V5),"",FALSE))</f>
+        <f t="array" ref="O6">IF(X6="","",IF(AND(X6&lt;&gt;X$2:X5),"",FALSE))</f>
         <v/>
       </c>
       <c r="P6" s="1" t="str" cm="1">
-        <f t="array" ref="P6">IF(W6="","",IF(AND(W6&lt;&gt;W$2:W5),"",FALSE))</f>
+        <f t="array" ref="P6">IF(Y6="","",IF(AND(Y6&lt;&gt;Y$2:Y5),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q6" s="1" t="str" cm="1">
-        <f t="array" ref="Q6">IF(X6="","",IF(AND(X6&lt;&gt;X$2:X5),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R6" s="1" t="str">
+        <f t="array" ref="Q6">IF(Z6="","",IF(AND(Z6&lt;&gt;Z$2:Z5),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R6" s="1" t="str" cm="1">
+        <f t="array" ref="R6">IF(F6="","",IF(AND(F6&lt;&gt;F$2:F5),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S6" s="1" t="str" cm="1">
+        <f t="array" ref="S6">IF(AA6="","",IF(AND(AA6&lt;&gt;AA$2:AA5),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T6" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S6" s="1" t="str">
+      <c r="U6" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U6" s="1" t="str">
+      <c r="V6" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V6" s="1" t="str">
+      <c r="X6" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W6" s="1" t="str">
+      <c r="Y6" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X6" s="1" t="str">
+      <c r="Z6" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA6" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1767,57 +1815,66 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="L7" s="1" t="str">
-        <f>IF(F7="","",+VLOOKUP(F7,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
       <c r="M7" s="1" t="str">
-        <f>IF(G7="","",+VLOOKUP(G7,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N7" s="1" t="str" cm="1">
-        <f t="array" ref="N7">IF(U7="","",IF(AND(U7&lt;&gt;U$2:U6),"",FALSE))</f>
+        <f>IF(G7="","",+VLOOKUP(G7,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f>IF(H7="","",+VLOOKUP(H7,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O7" s="1" t="str" cm="1">
-        <f t="array" ref="O7">IF(V7="","",IF(AND(V7&lt;&gt;V$2:V6),"",FALSE))</f>
+        <f t="array" ref="O7">IF(X7="","",IF(AND(X7&lt;&gt;X$2:X6),"",FALSE))</f>
         <v/>
       </c>
       <c r="P7" s="1" t="str" cm="1">
-        <f t="array" ref="P7">IF(W7="","",IF(AND(W7&lt;&gt;W$2:W6),"",FALSE))</f>
+        <f t="array" ref="P7">IF(Y7="","",IF(AND(Y7&lt;&gt;Y$2:Y6),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q7" s="1" t="str" cm="1">
-        <f t="array" ref="Q7">IF(X7="","",IF(AND(X7&lt;&gt;X$2:X6),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R7" s="1" t="str">
+        <f t="array" ref="Q7">IF(Z7="","",IF(AND(Z7&lt;&gt;Z$2:Z6),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R7" s="1" t="str" cm="1">
+        <f t="array" ref="R7">IF(F7="","",IF(AND(F7&lt;&gt;F$2:F6),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S7" s="1" t="str" cm="1">
+        <f t="array" ref="S7">IF(AA7="","",IF(AND(AA7&lt;&gt;AA$2:AA6),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T7" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S7" s="1" t="str">
+      <c r="U7" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U7" s="1" t="str">
+      <c r="V7" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V7" s="1" t="str">
+      <c r="X7" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W7" s="1" t="str">
+      <c r="Y7" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X7" s="1" t="str">
+      <c r="Z7" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA7" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1825,57 +1882,66 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="L8" s="1" t="str">
-        <f>IF(F8="","",+VLOOKUP(F8,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
       <c r="M8" s="1" t="str">
-        <f>IF(G8="","",+VLOOKUP(G8,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N8" s="1" t="str" cm="1">
-        <f t="array" ref="N8">IF(U8="","",IF(AND(U8&lt;&gt;U$2:U7),"",FALSE))</f>
+        <f>IF(G8="","",+VLOOKUP(G8,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N8" s="1" t="str">
+        <f>IF(H8="","",+VLOOKUP(H8,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O8" s="1" t="str" cm="1">
-        <f t="array" ref="O8">IF(V8="","",IF(AND(V8&lt;&gt;V$2:V7),"",FALSE))</f>
+        <f t="array" ref="O8">IF(X8="","",IF(AND(X8&lt;&gt;X$2:X7),"",FALSE))</f>
         <v/>
       </c>
       <c r="P8" s="1" t="str" cm="1">
-        <f t="array" ref="P8">IF(W8="","",IF(AND(W8&lt;&gt;W$2:W7),"",FALSE))</f>
+        <f t="array" ref="P8">IF(Y8="","",IF(AND(Y8&lt;&gt;Y$2:Y7),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q8" s="1" t="str" cm="1">
-        <f t="array" ref="Q8">IF(X8="","",IF(AND(X8&lt;&gt;X$2:X7),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R8" s="1" t="str">
+        <f t="array" ref="Q8">IF(Z8="","",IF(AND(Z8&lt;&gt;Z$2:Z7),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R8" s="1" t="str" cm="1">
+        <f t="array" ref="R8">IF(F8="","",IF(AND(F8&lt;&gt;F$2:F7),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S8" s="1" t="str" cm="1">
+        <f t="array" ref="S8">IF(AA8="","",IF(AND(AA8&lt;&gt;AA$2:AA7),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T8" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S8" s="1" t="str">
+      <c r="U8" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U8" s="1" t="str">
+      <c r="V8" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V8" s="1" t="str">
+      <c r="X8" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W8" s="1" t="str">
+      <c r="Y8" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X8" s="1" t="str">
+      <c r="Z8" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA8" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1883,57 +1949,66 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="L9" s="1" t="str">
-        <f>IF(F9="","",+VLOOKUP(F9,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
       <c r="M9" s="1" t="str">
-        <f>IF(G9="","",+VLOOKUP(G9,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N9" s="1" t="str" cm="1">
-        <f t="array" ref="N9">IF(U9="","",IF(AND(U9&lt;&gt;U$2:U8),"",FALSE))</f>
+        <f>IF(G9="","",+VLOOKUP(G9,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N9" s="1" t="str">
+        <f>IF(H9="","",+VLOOKUP(H9,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O9" s="1" t="str" cm="1">
-        <f t="array" ref="O9">IF(V9="","",IF(AND(V9&lt;&gt;V$2:V8),"",FALSE))</f>
+        <f t="array" ref="O9">IF(X9="","",IF(AND(X9&lt;&gt;X$2:X8),"",FALSE))</f>
         <v/>
       </c>
       <c r="P9" s="1" t="str" cm="1">
-        <f t="array" ref="P9">IF(W9="","",IF(AND(W9&lt;&gt;W$2:W8),"",FALSE))</f>
+        <f t="array" ref="P9">IF(Y9="","",IF(AND(Y9&lt;&gt;Y$2:Y8),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q9" s="1" t="str" cm="1">
-        <f t="array" ref="Q9">IF(X9="","",IF(AND(X9&lt;&gt;X$2:X8),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R9" s="1" t="str">
+        <f t="array" ref="Q9">IF(Z9="","",IF(AND(Z9&lt;&gt;Z$2:Z8),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R9" s="1" t="str" cm="1">
+        <f t="array" ref="R9">IF(F9="","",IF(AND(F9&lt;&gt;F$2:F8),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S9" s="1" t="str" cm="1">
+        <f t="array" ref="S9">IF(AA9="","",IF(AND(AA9&lt;&gt;AA$2:AA8),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T9" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S9" s="1" t="str">
+      <c r="U9" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U9" s="1" t="str">
+      <c r="V9" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V9" s="1" t="str">
+      <c r="X9" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W9" s="1" t="str">
+      <c r="Y9" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X9" s="1" t="str">
+      <c r="Z9" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA9" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1941,57 +2016,66 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-      <c r="L10" s="1" t="str">
-        <f>IF(F10="","",+VLOOKUP(F10,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
       <c r="M10" s="1" t="str">
-        <f>IF(G10="","",+VLOOKUP(G10,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N10" s="1" t="str" cm="1">
-        <f t="array" ref="N10">IF(U10="","",IF(AND(U10&lt;&gt;U$2:U9),"",FALSE))</f>
+        <f>IF(G10="","",+VLOOKUP(G10,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f>IF(H10="","",+VLOOKUP(H10,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O10" s="1" t="str" cm="1">
-        <f t="array" ref="O10">IF(V10="","",IF(AND(V10&lt;&gt;V$2:V9),"",FALSE))</f>
+        <f t="array" ref="O10">IF(X10="","",IF(AND(X10&lt;&gt;X$2:X9),"",FALSE))</f>
         <v/>
       </c>
       <c r="P10" s="1" t="str" cm="1">
-        <f t="array" ref="P10">IF(W10="","",IF(AND(W10&lt;&gt;W$2:W9),"",FALSE))</f>
+        <f t="array" ref="P10">IF(Y10="","",IF(AND(Y10&lt;&gt;Y$2:Y9),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q10" s="1" t="str" cm="1">
-        <f t="array" ref="Q10">IF(X10="","",IF(AND(X10&lt;&gt;X$2:X9),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R10" s="1" t="str">
+        <f t="array" ref="Q10">IF(Z10="","",IF(AND(Z10&lt;&gt;Z$2:Z9),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R10" s="1" t="str" cm="1">
+        <f t="array" ref="R10">IF(F10="","",IF(AND(F10&lt;&gt;F$2:F9),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S10" s="1" t="str" cm="1">
+        <f t="array" ref="S10">IF(AA10="","",IF(AND(AA10&lt;&gt;AA$2:AA9),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T10" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S10" s="1" t="str">
+      <c r="U10" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U10" s="1" t="str">
+      <c r="V10" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V10" s="1" t="str">
+      <c r="X10" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W10" s="1" t="str">
+      <c r="Y10" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X10" s="1" t="str">
+      <c r="Z10" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA10" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1999,57 +2083,66 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
-      <c r="L11" s="1" t="str">
-        <f>IF(F11="","",+VLOOKUP(F11,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
       <c r="M11" s="1" t="str">
-        <f>IF(G11="","",+VLOOKUP(G11,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N11" s="1" t="str" cm="1">
-        <f t="array" ref="N11">IF(U11="","",IF(AND(U11&lt;&gt;U$2:U10),"",FALSE))</f>
+        <f>IF(G11="","",+VLOOKUP(G11,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N11" s="1" t="str">
+        <f>IF(H11="","",+VLOOKUP(H11,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O11" s="1" t="str" cm="1">
-        <f t="array" ref="O11">IF(V11="","",IF(AND(V11&lt;&gt;V$2:V10),"",FALSE))</f>
+        <f t="array" ref="O11">IF(X11="","",IF(AND(X11&lt;&gt;X$2:X10),"",FALSE))</f>
         <v/>
       </c>
       <c r="P11" s="1" t="str" cm="1">
-        <f t="array" ref="P11">IF(W11="","",IF(AND(W11&lt;&gt;W$2:W10),"",FALSE))</f>
+        <f t="array" ref="P11">IF(Y11="","",IF(AND(Y11&lt;&gt;Y$2:Y10),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q11" s="1" t="str" cm="1">
-        <f t="array" ref="Q11">IF(X11="","",IF(AND(X11&lt;&gt;X$2:X10),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R11" s="1" t="str">
+        <f t="array" ref="Q11">IF(Z11="","",IF(AND(Z11&lt;&gt;Z$2:Z10),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R11" s="1" t="str" cm="1">
+        <f t="array" ref="R11">IF(F11="","",IF(AND(F11&lt;&gt;F$2:F10),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S11" s="1" t="str" cm="1">
+        <f t="array" ref="S11">IF(AA11="","",IF(AND(AA11&lt;&gt;AA$2:AA10),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T11" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S11" s="1" t="str">
+      <c r="U11" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U11" s="1" t="str">
+      <c r="V11" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V11" s="1" t="str">
+      <c r="X11" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W11" s="1" t="str">
+      <c r="Y11" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X11" s="1" t="str">
+      <c r="Z11" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA11" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -2057,57 +2150,66 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
-      <c r="L12" s="1" t="str">
-        <f>IF(F12="","",+VLOOKUP(F12,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
       <c r="M12" s="1" t="str">
-        <f>IF(G12="","",+VLOOKUP(G12,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N12" s="1" t="str" cm="1">
-        <f t="array" ref="N12">IF(U12="","",IF(AND(U12&lt;&gt;U$2:U11),"",FALSE))</f>
+        <f>IF(G12="","",+VLOOKUP(G12,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N12" s="1" t="str">
+        <f>IF(H12="","",+VLOOKUP(H12,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O12" s="1" t="str" cm="1">
-        <f t="array" ref="O12">IF(V12="","",IF(AND(V12&lt;&gt;V$2:V11),"",FALSE))</f>
+        <f t="array" ref="O12">IF(X12="","",IF(AND(X12&lt;&gt;X$2:X11),"",FALSE))</f>
         <v/>
       </c>
       <c r="P12" s="1" t="str" cm="1">
-        <f t="array" ref="P12">IF(W12="","",IF(AND(W12&lt;&gt;W$2:W11),"",FALSE))</f>
+        <f t="array" ref="P12">IF(Y12="","",IF(AND(Y12&lt;&gt;Y$2:Y11),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q12" s="1" t="str" cm="1">
-        <f t="array" ref="Q12">IF(X12="","",IF(AND(X12&lt;&gt;X$2:X11),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R12" s="1" t="str">
+        <f t="array" ref="Q12">IF(Z12="","",IF(AND(Z12&lt;&gt;Z$2:Z11),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R12" s="1" t="str" cm="1">
+        <f t="array" ref="R12">IF(F12="","",IF(AND(F12&lt;&gt;F$2:F11),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S12" s="1" t="str" cm="1">
+        <f t="array" ref="S12">IF(AA12="","",IF(AND(AA12&lt;&gt;AA$2:AA11),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T12" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S12" s="1" t="str">
+      <c r="U12" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U12" s="1" t="str">
+      <c r="V12" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V12" s="1" t="str">
+      <c r="X12" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W12" s="1" t="str">
+      <c r="Y12" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X12" s="1" t="str">
+      <c r="Z12" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA12" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2115,57 +2217,66 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
-      <c r="L13" s="1" t="str">
-        <f>IF(F13="","",+VLOOKUP(F13,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="7"/>
       <c r="M13" s="1" t="str">
-        <f>IF(G13="","",+VLOOKUP(G13,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N13" s="1" t="str" cm="1">
-        <f t="array" ref="N13">IF(U13="","",IF(AND(U13&lt;&gt;U$2:U12),"",FALSE))</f>
+        <f>IF(G13="","",+VLOOKUP(G13,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N13" s="1" t="str">
+        <f>IF(H13="","",+VLOOKUP(H13,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O13" s="1" t="str" cm="1">
-        <f t="array" ref="O13">IF(V13="","",IF(AND(V13&lt;&gt;V$2:V12),"",FALSE))</f>
+        <f t="array" ref="O13">IF(X13="","",IF(AND(X13&lt;&gt;X$2:X12),"",FALSE))</f>
         <v/>
       </c>
       <c r="P13" s="1" t="str" cm="1">
-        <f t="array" ref="P13">IF(W13="","",IF(AND(W13&lt;&gt;W$2:W12),"",FALSE))</f>
+        <f t="array" ref="P13">IF(Y13="","",IF(AND(Y13&lt;&gt;Y$2:Y12),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q13" s="1" t="str" cm="1">
-        <f t="array" ref="Q13">IF(X13="","",IF(AND(X13&lt;&gt;X$2:X12),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R13" s="1" t="str">
+        <f t="array" ref="Q13">IF(Z13="","",IF(AND(Z13&lt;&gt;Z$2:Z12),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R13" s="1" t="str" cm="1">
+        <f t="array" ref="R13">IF(F13="","",IF(AND(F13&lt;&gt;F$2:F12),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S13" s="1" t="str" cm="1">
+        <f t="array" ref="S13">IF(AA13="","",IF(AND(AA13&lt;&gt;AA$2:AA12),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T13" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S13" s="1" t="str">
+      <c r="U13" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U13" s="1" t="str">
+      <c r="V13" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V13" s="1" t="str">
+      <c r="X13" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W13" s="1" t="str">
+      <c r="Y13" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X13" s="1" t="str">
+      <c r="Z13" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA13" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2173,57 +2284,66 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
-      <c r="L14" s="1" t="str">
-        <f>IF(F14="","",+VLOOKUP(F14,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
       <c r="M14" s="1" t="str">
-        <f>IF(G14="","",+VLOOKUP(G14,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N14" s="1" t="str" cm="1">
-        <f t="array" ref="N14">IF(U14="","",IF(AND(U14&lt;&gt;U$2:U13),"",FALSE))</f>
+        <f>IF(G14="","",+VLOOKUP(G14,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N14" s="1" t="str">
+        <f>IF(H14="","",+VLOOKUP(H14,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O14" s="1" t="str" cm="1">
-        <f t="array" ref="O14">IF(V14="","",IF(AND(V14&lt;&gt;V$2:V13),"",FALSE))</f>
+        <f t="array" ref="O14">IF(X14="","",IF(AND(X14&lt;&gt;X$2:X13),"",FALSE))</f>
         <v/>
       </c>
       <c r="P14" s="1" t="str" cm="1">
-        <f t="array" ref="P14">IF(W14="","",IF(AND(W14&lt;&gt;W$2:W13),"",FALSE))</f>
+        <f t="array" ref="P14">IF(Y14="","",IF(AND(Y14&lt;&gt;Y$2:Y13),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q14" s="1" t="str" cm="1">
-        <f t="array" ref="Q14">IF(X14="","",IF(AND(X14&lt;&gt;X$2:X13),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R14" s="1" t="str">
+        <f t="array" ref="Q14">IF(Z14="","",IF(AND(Z14&lt;&gt;Z$2:Z13),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R14" s="1" t="str" cm="1">
+        <f t="array" ref="R14">IF(F14="","",IF(AND(F14&lt;&gt;F$2:F13),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S14" s="1" t="str" cm="1">
+        <f t="array" ref="S14">IF(AA14="","",IF(AND(AA14&lt;&gt;AA$2:AA13),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T14" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S14" s="1" t="str">
+      <c r="U14" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U14" s="1" t="str">
+      <c r="V14" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V14" s="1" t="str">
+      <c r="X14" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W14" s="1" t="str">
+      <c r="Y14" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X14" s="1" t="str">
+      <c r="Z14" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA14" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2231,57 +2351,66 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="7"/>
-      <c r="L15" s="1" t="str">
-        <f>IF(F15="","",+VLOOKUP(F15,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="7"/>
       <c r="M15" s="1" t="str">
-        <f>IF(G15="","",+VLOOKUP(G15,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N15" s="1" t="str" cm="1">
-        <f t="array" ref="N15">IF(U15="","",IF(AND(U15&lt;&gt;U$2:U14),"",FALSE))</f>
+        <f>IF(G15="","",+VLOOKUP(G15,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N15" s="1" t="str">
+        <f>IF(H15="","",+VLOOKUP(H15,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O15" s="1" t="str" cm="1">
-        <f t="array" ref="O15">IF(V15="","",IF(AND(V15&lt;&gt;V$2:V14),"",FALSE))</f>
+        <f t="array" ref="O15">IF(X15="","",IF(AND(X15&lt;&gt;X$2:X14),"",FALSE))</f>
         <v/>
       </c>
       <c r="P15" s="1" t="str" cm="1">
-        <f t="array" ref="P15">IF(W15="","",IF(AND(W15&lt;&gt;W$2:W14),"",FALSE))</f>
+        <f t="array" ref="P15">IF(Y15="","",IF(AND(Y15&lt;&gt;Y$2:Y14),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q15" s="1" t="str" cm="1">
-        <f t="array" ref="Q15">IF(X15="","",IF(AND(X15&lt;&gt;X$2:X14),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R15" s="1" t="str">
+        <f t="array" ref="Q15">IF(Z15="","",IF(AND(Z15&lt;&gt;Z$2:Z14),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R15" s="1" t="str" cm="1">
+        <f t="array" ref="R15">IF(F15="","",IF(AND(F15&lt;&gt;F$2:F14),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S15" s="1" t="str" cm="1">
+        <f t="array" ref="S15">IF(AA15="","",IF(AND(AA15&lt;&gt;AA$2:AA14),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T15" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S15" s="1" t="str">
+      <c r="U15" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U15" s="1" t="str">
+      <c r="V15" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V15" s="1" t="str">
+      <c r="X15" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W15" s="1" t="str">
+      <c r="Y15" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X15" s="1" t="str">
+      <c r="Z15" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA15" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2289,57 +2418,66 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
-      <c r="L16" s="1" t="str">
-        <f>IF(F16="","",+VLOOKUP(F16,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="7"/>
       <c r="M16" s="1" t="str">
-        <f>IF(G16="","",+VLOOKUP(G16,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N16" s="1" t="str" cm="1">
-        <f t="array" ref="N16">IF(U16="","",IF(AND(U16&lt;&gt;U$2:U15),"",FALSE))</f>
+        <f>IF(G16="","",+VLOOKUP(G16,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N16" s="1" t="str">
+        <f>IF(H16="","",+VLOOKUP(H16,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O16" s="1" t="str" cm="1">
-        <f t="array" ref="O16">IF(V16="","",IF(AND(V16&lt;&gt;V$2:V15),"",FALSE))</f>
+        <f t="array" ref="O16">IF(X16="","",IF(AND(X16&lt;&gt;X$2:X15),"",FALSE))</f>
         <v/>
       </c>
       <c r="P16" s="1" t="str" cm="1">
-        <f t="array" ref="P16">IF(W16="","",IF(AND(W16&lt;&gt;W$2:W15),"",FALSE))</f>
+        <f t="array" ref="P16">IF(Y16="","",IF(AND(Y16&lt;&gt;Y$2:Y15),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q16" s="1" t="str" cm="1">
-        <f t="array" ref="Q16">IF(X16="","",IF(AND(X16&lt;&gt;X$2:X15),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R16" s="1" t="str">
+        <f t="array" ref="Q16">IF(Z16="","",IF(AND(Z16&lt;&gt;Z$2:Z15),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R16" s="1" t="str" cm="1">
+        <f t="array" ref="R16">IF(F16="","",IF(AND(F16&lt;&gt;F$2:F15),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S16" s="1" t="str" cm="1">
+        <f t="array" ref="S16">IF(AA16="","",IF(AND(AA16&lt;&gt;AA$2:AA15),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T16" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S16" s="1" t="str">
+      <c r="U16" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U16" s="1" t="str">
+      <c r="V16" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V16" s="1" t="str">
+      <c r="X16" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W16" s="1" t="str">
+      <c r="Y16" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X16" s="1" t="str">
+      <c r="Z16" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA16" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2347,57 +2485,66 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="7"/>
-      <c r="L17" s="1" t="str">
-        <f>IF(F17="","",+VLOOKUP(F17,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="7"/>
       <c r="M17" s="1" t="str">
-        <f>IF(G17="","",+VLOOKUP(G17,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N17" s="1" t="str" cm="1">
-        <f t="array" ref="N17">IF(U17="","",IF(AND(U17&lt;&gt;U$2:U16),"",FALSE))</f>
+        <f>IF(G17="","",+VLOOKUP(G17,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N17" s="1" t="str">
+        <f>IF(H17="","",+VLOOKUP(H17,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O17" s="1" t="str" cm="1">
-        <f t="array" ref="O17">IF(V17="","",IF(AND(V17&lt;&gt;V$2:V16),"",FALSE))</f>
+        <f t="array" ref="O17">IF(X17="","",IF(AND(X17&lt;&gt;X$2:X16),"",FALSE))</f>
         <v/>
       </c>
       <c r="P17" s="1" t="str" cm="1">
-        <f t="array" ref="P17">IF(W17="","",IF(AND(W17&lt;&gt;W$2:W16),"",FALSE))</f>
+        <f t="array" ref="P17">IF(Y17="","",IF(AND(Y17&lt;&gt;Y$2:Y16),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q17" s="1" t="str" cm="1">
-        <f t="array" ref="Q17">IF(X17="","",IF(AND(X17&lt;&gt;X$2:X16),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R17" s="1" t="str">
+        <f t="array" ref="Q17">IF(Z17="","",IF(AND(Z17&lt;&gt;Z$2:Z16),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R17" s="1" t="str" cm="1">
+        <f t="array" ref="R17">IF(F17="","",IF(AND(F17&lt;&gt;F$2:F16),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S17" s="1" t="str" cm="1">
+        <f t="array" ref="S17">IF(AA17="","",IF(AND(AA17&lt;&gt;AA$2:AA16),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T17" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S17" s="1" t="str">
+      <c r="U17" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U17" s="1" t="str">
+      <c r="V17" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V17" s="1" t="str">
+      <c r="X17" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W17" s="1" t="str">
+      <c r="Y17" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X17" s="1" t="str">
+      <c r="Z17" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA17" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -2405,57 +2552,66 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
-      <c r="L18" s="1" t="str">
-        <f>IF(F18="","",+VLOOKUP(F18,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
       <c r="M18" s="1" t="str">
-        <f>IF(G18="","",+VLOOKUP(G18,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N18" s="1" t="str" cm="1">
-        <f t="array" ref="N18">IF(U18="","",IF(AND(U18&lt;&gt;U$2:U17),"",FALSE))</f>
+        <f>IF(G18="","",+VLOOKUP(G18,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N18" s="1" t="str">
+        <f>IF(H18="","",+VLOOKUP(H18,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O18" s="1" t="str" cm="1">
-        <f t="array" ref="O18">IF(V18="","",IF(AND(V18&lt;&gt;V$2:V17),"",FALSE))</f>
+        <f t="array" ref="O18">IF(X18="","",IF(AND(X18&lt;&gt;X$2:X17),"",FALSE))</f>
         <v/>
       </c>
       <c r="P18" s="1" t="str" cm="1">
-        <f t="array" ref="P18">IF(W18="","",IF(AND(W18&lt;&gt;W$2:W17),"",FALSE))</f>
+        <f t="array" ref="P18">IF(Y18="","",IF(AND(Y18&lt;&gt;Y$2:Y17),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q18" s="1" t="str" cm="1">
-        <f t="array" ref="Q18">IF(X18="","",IF(AND(X18&lt;&gt;X$2:X17),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R18" s="1" t="str">
+        <f t="array" ref="Q18">IF(Z18="","",IF(AND(Z18&lt;&gt;Z$2:Z17),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R18" s="1" t="str" cm="1">
+        <f t="array" ref="R18">IF(F18="","",IF(AND(F18&lt;&gt;F$2:F17),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S18" s="1" t="str" cm="1">
+        <f t="array" ref="S18">IF(AA18="","",IF(AND(AA18&lt;&gt;AA$2:AA17),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T18" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S18" s="1" t="str">
+      <c r="U18" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U18" s="1" t="str">
+      <c r="V18" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V18" s="1" t="str">
+      <c r="X18" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W18" s="1" t="str">
+      <c r="Y18" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X18" s="1" t="str">
+      <c r="Z18" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA18" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2463,57 +2619,66 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="7"/>
-      <c r="L19" s="1" t="str">
-        <f>IF(F19="","",+VLOOKUP(F19,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
       <c r="M19" s="1" t="str">
-        <f>IF(G19="","",+VLOOKUP(G19,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N19" s="1" t="str" cm="1">
-        <f t="array" ref="N19">IF(U19="","",IF(AND(U19&lt;&gt;U$2:U18),"",FALSE))</f>
+        <f>IF(G19="","",+VLOOKUP(G19,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N19" s="1" t="str">
+        <f>IF(H19="","",+VLOOKUP(H19,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O19" s="1" t="str" cm="1">
-        <f t="array" ref="O19">IF(V19="","",IF(AND(V19&lt;&gt;V$2:V18),"",FALSE))</f>
+        <f t="array" ref="O19">IF(X19="","",IF(AND(X19&lt;&gt;X$2:X18),"",FALSE))</f>
         <v/>
       </c>
       <c r="P19" s="1" t="str" cm="1">
-        <f t="array" ref="P19">IF(W19="","",IF(AND(W19&lt;&gt;W$2:W18),"",FALSE))</f>
+        <f t="array" ref="P19">IF(Y19="","",IF(AND(Y19&lt;&gt;Y$2:Y18),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q19" s="1" t="str" cm="1">
-        <f t="array" ref="Q19">IF(X19="","",IF(AND(X19&lt;&gt;X$2:X18),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R19" s="1" t="str">
+        <f t="array" ref="Q19">IF(Z19="","",IF(AND(Z19&lt;&gt;Z$2:Z18),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R19" s="1" t="str" cm="1">
+        <f t="array" ref="R19">IF(F19="","",IF(AND(F19&lt;&gt;F$2:F18),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S19" s="1" t="str" cm="1">
+        <f t="array" ref="S19">IF(AA19="","",IF(AND(AA19&lt;&gt;AA$2:AA18),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T19" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S19" s="1" t="str">
+      <c r="U19" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U19" s="1" t="str">
+      <c r="V19" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V19" s="1" t="str">
+      <c r="X19" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W19" s="1" t="str">
+      <c r="Y19" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X19" s="1" t="str">
+      <c r="Z19" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA19" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -2521,57 +2686,66 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
-      <c r="L20" s="1" t="str">
-        <f>IF(F20="","",+VLOOKUP(F20,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="7"/>
       <c r="M20" s="1" t="str">
-        <f>IF(G20="","",+VLOOKUP(G20,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N20" s="1" t="str" cm="1">
-        <f t="array" ref="N20">IF(U20="","",IF(AND(U20&lt;&gt;U$2:U19),"",FALSE))</f>
+        <f>IF(G20="","",+VLOOKUP(G20,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N20" s="1" t="str">
+        <f>IF(H20="","",+VLOOKUP(H20,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O20" s="1" t="str" cm="1">
-        <f t="array" ref="O20">IF(V20="","",IF(AND(V20&lt;&gt;V$2:V19),"",FALSE))</f>
+        <f t="array" ref="O20">IF(X20="","",IF(AND(X20&lt;&gt;X$2:X19),"",FALSE))</f>
         <v/>
       </c>
       <c r="P20" s="1" t="str" cm="1">
-        <f t="array" ref="P20">IF(W20="","",IF(AND(W20&lt;&gt;W$2:W19),"",FALSE))</f>
+        <f t="array" ref="P20">IF(Y20="","",IF(AND(Y20&lt;&gt;Y$2:Y19),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q20" s="1" t="str" cm="1">
-        <f t="array" ref="Q20">IF(X20="","",IF(AND(X20&lt;&gt;X$2:X19),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R20" s="1" t="str">
+        <f t="array" ref="Q20">IF(Z20="","",IF(AND(Z20&lt;&gt;Z$2:Z19),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R20" s="1" t="str" cm="1">
+        <f t="array" ref="R20">IF(F20="","",IF(AND(F20&lt;&gt;F$2:F19),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S20" s="1" t="str" cm="1">
+        <f t="array" ref="S20">IF(AA20="","",IF(AND(AA20&lt;&gt;AA$2:AA19),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T20" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S20" s="1" t="str">
+      <c r="U20" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U20" s="1" t="str">
+      <c r="V20" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V20" s="1" t="str">
+      <c r="X20" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W20" s="1" t="str">
+      <c r="Y20" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X20" s="1" t="str">
+      <c r="Z20" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA20" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -2579,57 +2753,66 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="7"/>
-      <c r="L21" s="1" t="str">
-        <f>IF(F21="","",+VLOOKUP(F21,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7"/>
       <c r="M21" s="1" t="str">
-        <f>IF(G21="","",+VLOOKUP(G21,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N21" s="1" t="str" cm="1">
-        <f t="array" ref="N21">IF(U21="","",IF(AND(U21&lt;&gt;U$2:U20),"",FALSE))</f>
+        <f>IF(G21="","",+VLOOKUP(G21,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N21" s="1" t="str">
+        <f>IF(H21="","",+VLOOKUP(H21,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O21" s="1" t="str" cm="1">
-        <f t="array" ref="O21">IF(V21="","",IF(AND(V21&lt;&gt;V$2:V20),"",FALSE))</f>
+        <f t="array" ref="O21">IF(X21="","",IF(AND(X21&lt;&gt;X$2:X20),"",FALSE))</f>
         <v/>
       </c>
       <c r="P21" s="1" t="str" cm="1">
-        <f t="array" ref="P21">IF(W21="","",IF(AND(W21&lt;&gt;W$2:W20),"",FALSE))</f>
+        <f t="array" ref="P21">IF(Y21="","",IF(AND(Y21&lt;&gt;Y$2:Y20),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q21" s="1" t="str" cm="1">
-        <f t="array" ref="Q21">IF(X21="","",IF(AND(X21&lt;&gt;X$2:X20),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R21" s="1" t="str">
+        <f t="array" ref="Q21">IF(Z21="","",IF(AND(Z21&lt;&gt;Z$2:Z20),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R21" s="1" t="str" cm="1">
+        <f t="array" ref="R21">IF(F21="","",IF(AND(F21&lt;&gt;F$2:F20),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S21" s="1" t="str" cm="1">
+        <f t="array" ref="S21">IF(AA21="","",IF(AND(AA21&lt;&gt;AA$2:AA20),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T21" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S21" s="1" t="str">
+      <c r="U21" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U21" s="1" t="str">
+      <c r="V21" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V21" s="1" t="str">
+      <c r="X21" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W21" s="1" t="str">
+      <c r="Y21" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X21" s="1" t="str">
+      <c r="Z21" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA21" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -2637,57 +2820,66 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
-      <c r="L22" s="1" t="str">
-        <f>IF(F22="","",+VLOOKUP(F22,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="7"/>
       <c r="M22" s="1" t="str">
-        <f>IF(G22="","",+VLOOKUP(G22,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N22" s="1" t="str" cm="1">
-        <f t="array" ref="N22">IF(U22="","",IF(AND(U22&lt;&gt;U$2:U21),"",FALSE))</f>
+        <f>IF(G22="","",+VLOOKUP(G22,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N22" s="1" t="str">
+        <f>IF(H22="","",+VLOOKUP(H22,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O22" s="1" t="str" cm="1">
-        <f t="array" ref="O22">IF(V22="","",IF(AND(V22&lt;&gt;V$2:V21),"",FALSE))</f>
+        <f t="array" ref="O22">IF(X22="","",IF(AND(X22&lt;&gt;X$2:X21),"",FALSE))</f>
         <v/>
       </c>
       <c r="P22" s="1" t="str" cm="1">
-        <f t="array" ref="P22">IF(W22="","",IF(AND(W22&lt;&gt;W$2:W21),"",FALSE))</f>
+        <f t="array" ref="P22">IF(Y22="","",IF(AND(Y22&lt;&gt;Y$2:Y21),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q22" s="1" t="str" cm="1">
-        <f t="array" ref="Q22">IF(X22="","",IF(AND(X22&lt;&gt;X$2:X21),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R22" s="1" t="str">
+        <f t="array" ref="Q22">IF(Z22="","",IF(AND(Z22&lt;&gt;Z$2:Z21),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R22" s="1" t="str" cm="1">
+        <f t="array" ref="R22">IF(F22="","",IF(AND(F22&lt;&gt;F$2:F21),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S22" s="1" t="str" cm="1">
+        <f t="array" ref="S22">IF(AA22="","",IF(AND(AA22&lt;&gt;AA$2:AA21),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T22" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S22" s="1" t="str">
+      <c r="U22" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U22" s="1" t="str">
+      <c r="V22" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V22" s="1" t="str">
+      <c r="X22" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W22" s="1" t="str">
+      <c r="Y22" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X22" s="1" t="str">
+      <c r="Z22" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA22" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -2695,57 +2887,66 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="7"/>
-      <c r="L23" s="1" t="str">
-        <f>IF(F23="","",+VLOOKUP(F23,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="7"/>
       <c r="M23" s="1" t="str">
-        <f>IF(G23="","",+VLOOKUP(G23,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N23" s="1" t="str" cm="1">
-        <f t="array" ref="N23">IF(U23="","",IF(AND(U23&lt;&gt;U$2:U22),"",FALSE))</f>
+        <f>IF(G23="","",+VLOOKUP(G23,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N23" s="1" t="str">
+        <f>IF(H23="","",+VLOOKUP(H23,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O23" s="1" t="str" cm="1">
-        <f t="array" ref="O23">IF(V23="","",IF(AND(V23&lt;&gt;V$2:V22),"",FALSE))</f>
+        <f t="array" ref="O23">IF(X23="","",IF(AND(X23&lt;&gt;X$2:X22),"",FALSE))</f>
         <v/>
       </c>
       <c r="P23" s="1" t="str" cm="1">
-        <f t="array" ref="P23">IF(W23="","",IF(AND(W23&lt;&gt;W$2:W22),"",FALSE))</f>
+        <f t="array" ref="P23">IF(Y23="","",IF(AND(Y23&lt;&gt;Y$2:Y22),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q23" s="1" t="str" cm="1">
-        <f t="array" ref="Q23">IF(X23="","",IF(AND(X23&lt;&gt;X$2:X22),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R23" s="1" t="str">
+        <f t="array" ref="Q23">IF(Z23="","",IF(AND(Z23&lt;&gt;Z$2:Z22),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R23" s="1" t="str" cm="1">
+        <f t="array" ref="R23">IF(F23="","",IF(AND(F23&lt;&gt;F$2:F22),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S23" s="1" t="str" cm="1">
+        <f t="array" ref="S23">IF(AA23="","",IF(AND(AA23&lt;&gt;AA$2:AA22),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T23" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S23" s="1" t="str">
+      <c r="U23" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U23" s="1" t="str">
+      <c r="V23" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V23" s="1" t="str">
+      <c r="X23" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W23" s="1" t="str">
+      <c r="Y23" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X23" s="1" t="str">
+      <c r="Z23" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA23" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -2753,57 +2954,66 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="7"/>
-      <c r="L24" s="1" t="str">
-        <f>IF(F24="","",+VLOOKUP(F24,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="7"/>
       <c r="M24" s="1" t="str">
-        <f>IF(G24="","",+VLOOKUP(G24,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N24" s="1" t="str" cm="1">
-        <f t="array" ref="N24">IF(U24="","",IF(AND(U24&lt;&gt;U$2:U23),"",FALSE))</f>
+        <f>IF(G24="","",+VLOOKUP(G24,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N24" s="1" t="str">
+        <f>IF(H24="","",+VLOOKUP(H24,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O24" s="1" t="str" cm="1">
-        <f t="array" ref="O24">IF(V24="","",IF(AND(V24&lt;&gt;V$2:V23),"",FALSE))</f>
+        <f t="array" ref="O24">IF(X24="","",IF(AND(X24&lt;&gt;X$2:X23),"",FALSE))</f>
         <v/>
       </c>
       <c r="P24" s="1" t="str" cm="1">
-        <f t="array" ref="P24">IF(W24="","",IF(AND(W24&lt;&gt;W$2:W23),"",FALSE))</f>
+        <f t="array" ref="P24">IF(Y24="","",IF(AND(Y24&lt;&gt;Y$2:Y23),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q24" s="1" t="str" cm="1">
-        <f t="array" ref="Q24">IF(X24="","",IF(AND(X24&lt;&gt;X$2:X23),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R24" s="1" t="str">
+        <f t="array" ref="Q24">IF(Z24="","",IF(AND(Z24&lt;&gt;Z$2:Z23),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R24" s="1" t="str" cm="1">
+        <f t="array" ref="R24">IF(F24="","",IF(AND(F24&lt;&gt;F$2:F23),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S24" s="1" t="str" cm="1">
+        <f t="array" ref="S24">IF(AA24="","",IF(AND(AA24&lt;&gt;AA$2:AA23),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T24" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S24" s="1" t="str">
+      <c r="U24" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U24" s="1" t="str">
+      <c r="V24" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V24" s="1" t="str">
+      <c r="X24" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W24" s="1" t="str">
+      <c r="Y24" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X24" s="1" t="str">
+      <c r="Z24" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA24" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -2811,57 +3021,66 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="7"/>
-      <c r="L25" s="1" t="str">
-        <f>IF(F25="","",+VLOOKUP(F25,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="7"/>
       <c r="M25" s="1" t="str">
-        <f>IF(G25="","",+VLOOKUP(G25,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N25" s="1" t="str" cm="1">
-        <f t="array" ref="N25">IF(U25="","",IF(AND(U25&lt;&gt;U$2:U24),"",FALSE))</f>
+        <f>IF(G25="","",+VLOOKUP(G25,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N25" s="1" t="str">
+        <f>IF(H25="","",+VLOOKUP(H25,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O25" s="1" t="str" cm="1">
-        <f t="array" ref="O25">IF(V25="","",IF(AND(V25&lt;&gt;V$2:V24),"",FALSE))</f>
+        <f t="array" ref="O25">IF(X25="","",IF(AND(X25&lt;&gt;X$2:X24),"",FALSE))</f>
         <v/>
       </c>
       <c r="P25" s="1" t="str" cm="1">
-        <f t="array" ref="P25">IF(W25="","",IF(AND(W25&lt;&gt;W$2:W24),"",FALSE))</f>
+        <f t="array" ref="P25">IF(Y25="","",IF(AND(Y25&lt;&gt;Y$2:Y24),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q25" s="1" t="str" cm="1">
-        <f t="array" ref="Q25">IF(X25="","",IF(AND(X25&lt;&gt;X$2:X24),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R25" s="1" t="str">
+        <f t="array" ref="Q25">IF(Z25="","",IF(AND(Z25&lt;&gt;Z$2:Z24),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R25" s="1" t="str" cm="1">
+        <f t="array" ref="R25">IF(F25="","",IF(AND(F25&lt;&gt;F$2:F24),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S25" s="1" t="str" cm="1">
+        <f t="array" ref="S25">IF(AA25="","",IF(AND(AA25&lt;&gt;AA$2:AA24),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T25" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S25" s="1" t="str">
+      <c r="U25" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U25" s="1" t="str">
+      <c r="V25" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V25" s="1" t="str">
+      <c r="X25" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W25" s="1" t="str">
+      <c r="Y25" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X25" s="1" t="str">
+      <c r="Z25" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA25" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -2869,57 +3088,66 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="7"/>
-      <c r="L26" s="1" t="str">
-        <f>IF(F26="","",+VLOOKUP(F26,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
       <c r="M26" s="1" t="str">
-        <f>IF(G26="","",+VLOOKUP(G26,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N26" s="1" t="str" cm="1">
-        <f t="array" ref="N26">IF(U26="","",IF(AND(U26&lt;&gt;U$2:U25),"",FALSE))</f>
+        <f>IF(G26="","",+VLOOKUP(G26,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N26" s="1" t="str">
+        <f>IF(H26="","",+VLOOKUP(H26,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O26" s="1" t="str" cm="1">
-        <f t="array" ref="O26">IF(V26="","",IF(AND(V26&lt;&gt;V$2:V25),"",FALSE))</f>
+        <f t="array" ref="O26">IF(X26="","",IF(AND(X26&lt;&gt;X$2:X25),"",FALSE))</f>
         <v/>
       </c>
       <c r="P26" s="1" t="str" cm="1">
-        <f t="array" ref="P26">IF(W26="","",IF(AND(W26&lt;&gt;W$2:W25),"",FALSE))</f>
+        <f t="array" ref="P26">IF(Y26="","",IF(AND(Y26&lt;&gt;Y$2:Y25),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q26" s="1" t="str" cm="1">
-        <f t="array" ref="Q26">IF(X26="","",IF(AND(X26&lt;&gt;X$2:X25),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R26" s="1" t="str">
+        <f t="array" ref="Q26">IF(Z26="","",IF(AND(Z26&lt;&gt;Z$2:Z25),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R26" s="1" t="str" cm="1">
+        <f t="array" ref="R26">IF(F26="","",IF(AND(F26&lt;&gt;F$2:F25),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S26" s="1" t="str" cm="1">
+        <f t="array" ref="S26">IF(AA26="","",IF(AND(AA26&lt;&gt;AA$2:AA25),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T26" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S26" s="1" t="str">
+      <c r="U26" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U26" s="1" t="str">
+      <c r="V26" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V26" s="1" t="str">
+      <c r="X26" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W26" s="1" t="str">
+      <c r="Y26" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X26" s="1" t="str">
+      <c r="Z26" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA26" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -2927,57 +3155,66 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="7"/>
-      <c r="L27" s="1" t="str">
-        <f>IF(F27="","",+VLOOKUP(F27,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="7"/>
       <c r="M27" s="1" t="str">
-        <f>IF(G27="","",+VLOOKUP(G27,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N27" s="1" t="str" cm="1">
-        <f t="array" ref="N27">IF(U27="","",IF(AND(U27&lt;&gt;U$2:U26),"",FALSE))</f>
+        <f>IF(G27="","",+VLOOKUP(G27,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N27" s="1" t="str">
+        <f>IF(H27="","",+VLOOKUP(H27,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O27" s="1" t="str" cm="1">
-        <f t="array" ref="O27">IF(V27="","",IF(AND(V27&lt;&gt;V$2:V26),"",FALSE))</f>
+        <f t="array" ref="O27">IF(X27="","",IF(AND(X27&lt;&gt;X$2:X26),"",FALSE))</f>
         <v/>
       </c>
       <c r="P27" s="1" t="str" cm="1">
-        <f t="array" ref="P27">IF(W27="","",IF(AND(W27&lt;&gt;W$2:W26),"",FALSE))</f>
+        <f t="array" ref="P27">IF(Y27="","",IF(AND(Y27&lt;&gt;Y$2:Y26),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q27" s="1" t="str" cm="1">
-        <f t="array" ref="Q27">IF(X27="","",IF(AND(X27&lt;&gt;X$2:X26),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R27" s="1" t="str">
+        <f t="array" ref="Q27">IF(Z27="","",IF(AND(Z27&lt;&gt;Z$2:Z26),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R27" s="1" t="str" cm="1">
+        <f t="array" ref="R27">IF(F27="","",IF(AND(F27&lt;&gt;F$2:F26),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S27" s="1" t="str" cm="1">
+        <f t="array" ref="S27">IF(AA27="","",IF(AND(AA27&lt;&gt;AA$2:AA26),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T27" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S27" s="1" t="str">
+      <c r="U27" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U27" s="1" t="str">
+      <c r="V27" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V27" s="1" t="str">
+      <c r="X27" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W27" s="1" t="str">
+      <c r="Y27" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X27" s="1" t="str">
+      <c r="Z27" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA27" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -2985,57 +3222,66 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
-      <c r="L28" s="1" t="str">
-        <f>IF(F28="","",+VLOOKUP(F28,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="7"/>
       <c r="M28" s="1" t="str">
-        <f>IF(G28="","",+VLOOKUP(G28,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N28" s="1" t="str" cm="1">
-        <f t="array" ref="N28">IF(U28="","",IF(AND(U28&lt;&gt;U$2:U27),"",FALSE))</f>
+        <f>IF(G28="","",+VLOOKUP(G28,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N28" s="1" t="str">
+        <f>IF(H28="","",+VLOOKUP(H28,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O28" s="1" t="str" cm="1">
-        <f t="array" ref="O28">IF(V28="","",IF(AND(V28&lt;&gt;V$2:V27),"",FALSE))</f>
+        <f t="array" ref="O28">IF(X28="","",IF(AND(X28&lt;&gt;X$2:X27),"",FALSE))</f>
         <v/>
       </c>
       <c r="P28" s="1" t="str" cm="1">
-        <f t="array" ref="P28">IF(W28="","",IF(AND(W28&lt;&gt;W$2:W27),"",FALSE))</f>
+        <f t="array" ref="P28">IF(Y28="","",IF(AND(Y28&lt;&gt;Y$2:Y27),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q28" s="1" t="str" cm="1">
-        <f t="array" ref="Q28">IF(X28="","",IF(AND(X28&lt;&gt;X$2:X27),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R28" s="1" t="str">
+        <f t="array" ref="Q28">IF(Z28="","",IF(AND(Z28&lt;&gt;Z$2:Z27),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R28" s="1" t="str" cm="1">
+        <f t="array" ref="R28">IF(F28="","",IF(AND(F28&lt;&gt;F$2:F27),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S28" s="1" t="str" cm="1">
+        <f t="array" ref="S28">IF(AA28="","",IF(AND(AA28&lt;&gt;AA$2:AA27),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T28" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S28" s="1" t="str">
+      <c r="U28" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U28" s="1" t="str">
+      <c r="V28" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V28" s="1" t="str">
+      <c r="X28" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W28" s="1" t="str">
+      <c r="Y28" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X28" s="1" t="str">
+      <c r="Z28" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA28" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -3043,57 +3289,66 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="7"/>
-      <c r="L29" s="1" t="str">
-        <f>IF(F29="","",+VLOOKUP(F29,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="7"/>
       <c r="M29" s="1" t="str">
-        <f>IF(G29="","",+VLOOKUP(G29,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N29" s="1" t="str" cm="1">
-        <f t="array" ref="N29">IF(U29="","",IF(AND(U29&lt;&gt;U$2:U28),"",FALSE))</f>
+        <f>IF(G29="","",+VLOOKUP(G29,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N29" s="1" t="str">
+        <f>IF(H29="","",+VLOOKUP(H29,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O29" s="1" t="str" cm="1">
-        <f t="array" ref="O29">IF(V29="","",IF(AND(V29&lt;&gt;V$2:V28),"",FALSE))</f>
+        <f t="array" ref="O29">IF(X29="","",IF(AND(X29&lt;&gt;X$2:X28),"",FALSE))</f>
         <v/>
       </c>
       <c r="P29" s="1" t="str" cm="1">
-        <f t="array" ref="P29">IF(W29="","",IF(AND(W29&lt;&gt;W$2:W28),"",FALSE))</f>
+        <f t="array" ref="P29">IF(Y29="","",IF(AND(Y29&lt;&gt;Y$2:Y28),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q29" s="1" t="str" cm="1">
-        <f t="array" ref="Q29">IF(X29="","",IF(AND(X29&lt;&gt;X$2:X28),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R29" s="1" t="str">
+        <f t="array" ref="Q29">IF(Z29="","",IF(AND(Z29&lt;&gt;Z$2:Z28),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R29" s="1" t="str" cm="1">
+        <f t="array" ref="R29">IF(F29="","",IF(AND(F29&lt;&gt;F$2:F28),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S29" s="1" t="str" cm="1">
+        <f t="array" ref="S29">IF(AA29="","",IF(AND(AA29&lt;&gt;AA$2:AA28),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T29" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S29" s="1" t="str">
+      <c r="U29" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U29" s="1" t="str">
+      <c r="V29" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V29" s="1" t="str">
+      <c r="X29" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W29" s="1" t="str">
+      <c r="Y29" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X29" s="1" t="str">
+      <c r="Z29" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA29" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -3101,57 +3356,66 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
-      <c r="L30" s="1" t="str">
-        <f>IF(F30="","",+VLOOKUP(F30,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="7"/>
       <c r="M30" s="1" t="str">
-        <f>IF(G30="","",+VLOOKUP(G30,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N30" s="1" t="str" cm="1">
-        <f t="array" ref="N30">IF(U30="","",IF(AND(U30&lt;&gt;U$2:U29),"",FALSE))</f>
+        <f>IF(G30="","",+VLOOKUP(G30,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N30" s="1" t="str">
+        <f>IF(H30="","",+VLOOKUP(H30,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O30" s="1" t="str" cm="1">
-        <f t="array" ref="O30">IF(V30="","",IF(AND(V30&lt;&gt;V$2:V29),"",FALSE))</f>
+        <f t="array" ref="O30">IF(X30="","",IF(AND(X30&lt;&gt;X$2:X29),"",FALSE))</f>
         <v/>
       </c>
       <c r="P30" s="1" t="str" cm="1">
-        <f t="array" ref="P30">IF(W30="","",IF(AND(W30&lt;&gt;W$2:W29),"",FALSE))</f>
+        <f t="array" ref="P30">IF(Y30="","",IF(AND(Y30&lt;&gt;Y$2:Y29),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q30" s="1" t="str" cm="1">
-        <f t="array" ref="Q30">IF(X30="","",IF(AND(X30&lt;&gt;X$2:X29),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R30" s="1" t="str">
+        <f t="array" ref="Q30">IF(Z30="","",IF(AND(Z30&lt;&gt;Z$2:Z29),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R30" s="1" t="str" cm="1">
+        <f t="array" ref="R30">IF(F30="","",IF(AND(F30&lt;&gt;F$2:F29),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S30" s="1" t="str" cm="1">
+        <f t="array" ref="S30">IF(AA30="","",IF(AND(AA30&lt;&gt;AA$2:AA29),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T30" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S30" s="1" t="str">
+      <c r="U30" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U30" s="1" t="str">
+      <c r="V30" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V30" s="1" t="str">
+      <c r="X30" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W30" s="1" t="str">
+      <c r="Y30" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X30" s="1" t="str">
+      <c r="Z30" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA30" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -3159,57 +3423,66 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="7"/>
-      <c r="L31" s="1" t="str">
-        <f>IF(F31="","",+VLOOKUP(F31,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="7"/>
       <c r="M31" s="1" t="str">
-        <f>IF(G31="","",+VLOOKUP(G31,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N31" s="1" t="str" cm="1">
-        <f t="array" ref="N31">IF(U31="","",IF(AND(U31&lt;&gt;U$2:U30),"",FALSE))</f>
+        <f>IF(G31="","",+VLOOKUP(G31,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N31" s="1" t="str">
+        <f>IF(H31="","",+VLOOKUP(H31,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O31" s="1" t="str" cm="1">
-        <f t="array" ref="O31">IF(V31="","",IF(AND(V31&lt;&gt;V$2:V30),"",FALSE))</f>
+        <f t="array" ref="O31">IF(X31="","",IF(AND(X31&lt;&gt;X$2:X30),"",FALSE))</f>
         <v/>
       </c>
       <c r="P31" s="1" t="str" cm="1">
-        <f t="array" ref="P31">IF(W31="","",IF(AND(W31&lt;&gt;W$2:W30),"",FALSE))</f>
+        <f t="array" ref="P31">IF(Y31="","",IF(AND(Y31&lt;&gt;Y$2:Y30),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q31" s="1" t="str" cm="1">
-        <f t="array" ref="Q31">IF(X31="","",IF(AND(X31&lt;&gt;X$2:X30),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R31" s="1" t="str">
+        <f t="array" ref="Q31">IF(Z31="","",IF(AND(Z31&lt;&gt;Z$2:Z30),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R31" s="1" t="str" cm="1">
+        <f t="array" ref="R31">IF(F31="","",IF(AND(F31&lt;&gt;F$2:F30),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S31" s="1" t="str" cm="1">
+        <f t="array" ref="S31">IF(AA31="","",IF(AND(AA31&lt;&gt;AA$2:AA30),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T31" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S31" s="1" t="str">
+      <c r="U31" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U31" s="1" t="str">
+      <c r="V31" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V31" s="1" t="str">
+      <c r="X31" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W31" s="1" t="str">
+      <c r="Y31" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X31" s="1" t="str">
+      <c r="Z31" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA31" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -3217,57 +3490,66 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="7"/>
-      <c r="L32" s="1" t="str">
-        <f>IF(F32="","",+VLOOKUP(F32,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="7"/>
       <c r="M32" s="1" t="str">
-        <f>IF(G32="","",+VLOOKUP(G32,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N32" s="1" t="str" cm="1">
-        <f t="array" ref="N32">IF(U32="","",IF(AND(U32&lt;&gt;U$2:U31),"",FALSE))</f>
+        <f>IF(G32="","",+VLOOKUP(G32,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N32" s="1" t="str">
+        <f>IF(H32="","",+VLOOKUP(H32,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O32" s="1" t="str" cm="1">
-        <f t="array" ref="O32">IF(V32="","",IF(AND(V32&lt;&gt;V$2:V31),"",FALSE))</f>
+        <f t="array" ref="O32">IF(X32="","",IF(AND(X32&lt;&gt;X$2:X31),"",FALSE))</f>
         <v/>
       </c>
       <c r="P32" s="1" t="str" cm="1">
-        <f t="array" ref="P32">IF(W32="","",IF(AND(W32&lt;&gt;W$2:W31),"",FALSE))</f>
+        <f t="array" ref="P32">IF(Y32="","",IF(AND(Y32&lt;&gt;Y$2:Y31),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q32" s="1" t="str" cm="1">
-        <f t="array" ref="Q32">IF(X32="","",IF(AND(X32&lt;&gt;X$2:X31),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R32" s="1" t="str">
+        <f t="array" ref="Q32">IF(Z32="","",IF(AND(Z32&lt;&gt;Z$2:Z31),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R32" s="1" t="str" cm="1">
+        <f t="array" ref="R32">IF(F32="","",IF(AND(F32&lt;&gt;F$2:F31),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S32" s="1" t="str" cm="1">
+        <f t="array" ref="S32">IF(AA32="","",IF(AND(AA32&lt;&gt;AA$2:AA31),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T32" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S32" s="1" t="str">
+      <c r="U32" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U32" s="1" t="str">
+      <c r="V32" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V32" s="1" t="str">
+      <c r="X32" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W32" s="1" t="str">
+      <c r="Y32" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X32" s="1" t="str">
+      <c r="Z32" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA32" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -3275,57 +3557,66 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="7"/>
-      <c r="L33" s="1" t="str">
-        <f>IF(F33="","",+VLOOKUP(F33,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="7"/>
       <c r="M33" s="1" t="str">
-        <f>IF(G33="","",+VLOOKUP(G33,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N33" s="1" t="str" cm="1">
-        <f t="array" ref="N33">IF(U33="","",IF(AND(U33&lt;&gt;U$2:U32),"",FALSE))</f>
+        <f>IF(G33="","",+VLOOKUP(G33,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N33" s="1" t="str">
+        <f>IF(H33="","",+VLOOKUP(H33,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O33" s="1" t="str" cm="1">
-        <f t="array" ref="O33">IF(V33="","",IF(AND(V33&lt;&gt;V$2:V32),"",FALSE))</f>
+        <f t="array" ref="O33">IF(X33="","",IF(AND(X33&lt;&gt;X$2:X32),"",FALSE))</f>
         <v/>
       </c>
       <c r="P33" s="1" t="str" cm="1">
-        <f t="array" ref="P33">IF(W33="","",IF(AND(W33&lt;&gt;W$2:W32),"",FALSE))</f>
+        <f t="array" ref="P33">IF(Y33="","",IF(AND(Y33&lt;&gt;Y$2:Y32),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q33" s="1" t="str" cm="1">
-        <f t="array" ref="Q33">IF(X33="","",IF(AND(X33&lt;&gt;X$2:X32),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R33" s="1" t="str">
+        <f t="array" ref="Q33">IF(Z33="","",IF(AND(Z33&lt;&gt;Z$2:Z32),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R33" s="1" t="str" cm="1">
+        <f t="array" ref="R33">IF(F33="","",IF(AND(F33&lt;&gt;F$2:F32),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S33" s="1" t="str" cm="1">
+        <f t="array" ref="S33">IF(AA33="","",IF(AND(AA33&lt;&gt;AA$2:AA32),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T33" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S33" s="1" t="str">
+      <c r="U33" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U33" s="1" t="str">
+      <c r="V33" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V33" s="1" t="str">
+      <c r="X33" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W33" s="1" t="str">
+      <c r="Y33" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X33" s="1" t="str">
+      <c r="Z33" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AA33" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -3333,71 +3624,80 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="7"/>
-      <c r="L34" s="1" t="str">
-        <f>IF(F34="","",+VLOOKUP(F34,'GST Code'!$A$1:$B$39,2,0))</f>
-        <v/>
-      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="7"/>
       <c r="M34" s="1" t="str">
-        <f>IF(G34="","",+VLOOKUP(G34,'STD Code'!$A$1:$B$150,2,0))</f>
-        <v/>
-      </c>
-      <c r="N34" s="1" t="str" cm="1">
-        <f t="array" ref="N34">IF(U34="","",IF(AND(U34&lt;&gt;U$2:U33),"",FALSE))</f>
+        <f>IF(G34="","",+VLOOKUP(G34,'GST Code'!$A$1:$B$39,2,0))</f>
+        <v/>
+      </c>
+      <c r="N34" s="1" t="str">
+        <f>IF(H34="","",+VLOOKUP(H34,'STD Code'!$A$1:$B$150,2,0))</f>
         <v/>
       </c>
       <c r="O34" s="1" t="str" cm="1">
-        <f t="array" ref="O34">IF(V34="","",IF(AND(V34&lt;&gt;V$2:V33),"",FALSE))</f>
+        <f t="array" ref="O34">IF(X34="","",IF(AND(X34&lt;&gt;X$2:X33),"",FALSE))</f>
         <v/>
       </c>
       <c r="P34" s="1" t="str" cm="1">
-        <f t="array" ref="P34">IF(W34="","",IF(AND(W34&lt;&gt;W$2:W33),"",FALSE))</f>
+        <f t="array" ref="P34">IF(Y34="","",IF(AND(Y34&lt;&gt;Y$2:Y33),"",FALSE))</f>
         <v/>
       </c>
       <c r="Q34" s="1" t="str" cm="1">
-        <f t="array" ref="Q34">IF(X34="","",IF(AND(X34&lt;&gt;X$2:X33),"",FALSE))</f>
-        <v/>
-      </c>
-      <c r="R34" s="1" t="str">
+        <f t="array" ref="Q34">IF(Z34="","",IF(AND(Z34&lt;&gt;Z$2:Z33),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="R34" s="1" t="str" cm="1">
+        <f t="array" ref="R34">IF(F34="","",IF(AND(F34&lt;&gt;F$2:F33),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="S34" s="1" t="str" cm="1">
+        <f t="array" ref="S34">IF(AA34="","",IF(AND(AA34&lt;&gt;AA$2:AA33),"",FALSE))</f>
+        <v/>
+      </c>
+      <c r="T34" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S34" s="1" t="str">
+      <c r="U34" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U34" s="1" t="str">
+      <c r="V34" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V34" s="1" t="str">
+      <c r="X34" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W34" s="1" t="str">
+      <c r="Y34" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X34" s="1" t="str">
+      <c r="Z34" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
+      <c r="AA34" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5BfmWedU/0A+qJKtbCCC3sYecFrAtxWeNKQpBS2GiAOjS9Wdc8TTHAAGzvZLc7Gr7nrJam+9mQds4nB+xeDTfA==" saltValue="oOLAq7x+uDZFoJBx+2Mx1Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2eaZQG3n2q9FFEmoLT1GNxoOd9W12/afLTf8gGQmurBPxAoGJxFaD24o4Rs0uMv9io1UC8NJxh7MDj3VtjGOlQ==" saltValue="loy2jeA1/rDEkFDl9KaGgA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:H1">
+  <conditionalFormatting sqref="A1:I1">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$I$2&gt;0</formula>
+      <formula>$J$2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:Q34">
+  <conditionalFormatting sqref="O3:S34">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pincode" error="Please enter Valid Pincode" promptTitle="Pincode" prompt="Enter 6 Digit Pin Code" sqref="H2:H34" xr:uid="{A868C3EC-6079-4370-AD7C-B251D546ECB1}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Pincode" error="Please enter Valid Pincode" promptTitle="Pincode" prompt="Enter 6 Digit Pin Code" sqref="I2:I34" xr:uid="{A868C3EC-6079-4370-AD7C-B251D546ECB1}">
       <formula1>100000</formula1>
       <formula2>999999</formula2>
     </dataValidation>
@@ -3405,8 +3705,8 @@
       <formula1>1000000000</formula1>
       <formula2>9999999999</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PAN Duplicate" error="Please dont Enter Duplicate PAN_x000a_" promptTitle="PAN Shoudl be Unique" prompt="Enter PAN of the organisation" sqref="C3:C34" xr:uid="{FC09F7C5-0873-4296-A17F-51C8B369F9EC}">
-      <formula1>IF(C3="",TRUE,IF(AND($C3&lt;&gt;$C$2:C2),TRUE,FALSE))</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PAN Duplicate" error="Please dont Enter Duplicate PAN_x000a_" promptTitle="PAN Shoudl be Unique" prompt="Enter PAN of the organisation" sqref="C5:C34" xr:uid="{FC09F7C5-0873-4296-A17F-51C8B369F9EC}">
+      <formula1>IF(C5="",TRUE,IF(AND($C5&lt;&gt;$C$2:C4),TRUE,FALSE))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3418,13 +3718,13 @@
           <x14:formula1>
             <xm:f>'GST Code'!$A$2:$A$39</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F34</xm:sqref>
+          <xm:sqref>G5:G34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2BE4BCE7-46C5-4E3F-9675-C78F3653DBD7}">
           <x14:formula1>
             <xm:f>'STD Code'!$A$2:$A$150</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G34</xm:sqref>
+          <xm:sqref>H5:H34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>